<commit_message>
2018 - latest greates Restriction data
</commit_message>
<xml_diff>
--- a/dataspace/2018/RestrictionsExport-07-16-20181.xlsx
+++ b/dataspace/2018/RestrictionsExport-07-16-20181.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
-  <workbookPr date1904="1" autoCompressPictures="0"/>
-  <bookViews>
-    <workbookView xWindow="6300" yWindow="500" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="RestrictionsExport-07-16-2018.t" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="RestrictionsExport-07-16-2018.t" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="219">
   <si>
     <t>ID</t>
   </si>
@@ -315,7 +307,70 @@
     <t>Peter Andolfatto</t>
   </si>
   <si>
-    <t>Fear_ Festis_ and FaÁade_ The Role of Privilege and Self-Curation in Educational Outcomes - Olivia Fiechter.xml</t>
+    <t>Why Should I Watch This Bloody Play_ The Ethical Potential of Pain in Performance_ by way of Sarah K - Nico Krell.xml</t>
+  </si>
+  <si>
+    <t>Nico Krell</t>
+  </si>
+  <si>
+    <t>Independent Study</t>
+  </si>
+  <si>
+    <t>Judith Hamera</t>
+  </si>
+  <si>
+    <t>The Struggle for Greater Autonomy_ Article 23 and the Development of the Pro-Democracy movement in H - Audrey Lee.xml</t>
+  </si>
+  <si>
+    <t>Audrey S. Lee</t>
+  </si>
+  <si>
+    <t>East Asian Studies</t>
+  </si>
+  <si>
+    <t>Anna M. Shields</t>
+  </si>
+  <si>
+    <t>Dopaminergic Activity Encodes and Modulates Freezing Behavior During Auditory Fear Extinction - Katherine Pizano.xml</t>
+  </si>
+  <si>
+    <t>Katherine Pizano</t>
+  </si>
+  <si>
+    <t>Molecular Biology</t>
+  </si>
+  <si>
+    <t>Ilana B. Witten</t>
+  </si>
+  <si>
+    <t>Temporospatial Dynamics of the Epithelial-Mesenchymal Transition in Cancer Metastasis_ - Daniel D. Liu.xml</t>
+  </si>
+  <si>
+    <t>Daniel D. Liu</t>
+  </si>
+  <si>
+    <t>Yibin Kang Lab</t>
+  </si>
+  <si>
+    <t>Missed Connections_ A Collection of Short Stories - Rebecca Kahn.xml</t>
+  </si>
+  <si>
+    <t>Rebecca N. Kahn</t>
+  </si>
+  <si>
+    <t>Daphne E. Kalotay</t>
+  </si>
+  <si>
+    <t>Photoswitchable Protein-Protein Interactions_ Engineering Light-Sensitive DARPins - Joshua Kim.xml</t>
+  </si>
+  <si>
+    <t>Joshua S. Kim</t>
+  </si>
+  <si>
+    <t>Toettcher</t>
+  </si>
+  <si>
+    <t>Fear_ Fetish_ and FaÁade_ The Role of Privilege and Self-Curation in Educational Outcomes - Olivia Fiechter.xml</t>
   </si>
   <si>
     <t>Olivia H. Fiechter</t>
@@ -325,72 +380,6 @@
   </si>
   <si>
     <t>Carolyn M. Rouse</t>
-  </si>
-  <si>
-    <t>Why Should I Watch This Bloody Play_ The Ethical Potential of Pain in Performance_ by way of Sarah K - Nico Krell.xml</t>
-  </si>
-  <si>
-    <t>Nico Krell</t>
-  </si>
-  <si>
-    <t>Independent Study</t>
-  </si>
-  <si>
-    <t>Judith Hamera</t>
-  </si>
-  <si>
-    <t>The Struggle for Greater Autonomy_ Article 23 and the Development of the Pro-Democracy movement in H - Audrey Lee.xml</t>
-  </si>
-  <si>
-    <t>Audrey S. Lee</t>
-  </si>
-  <si>
-    <t>East Asian Studies</t>
-  </si>
-  <si>
-    <t>Anna M. Shields</t>
-  </si>
-  <si>
-    <t>Dopaminergic Activity Encodes and Modulates Freezing Behavior During Auditory Fear Extinction - Katherine Pizano.xml</t>
-  </si>
-  <si>
-    <t>Katherine Pizano</t>
-  </si>
-  <si>
-    <t>Molecular Biology</t>
-  </si>
-  <si>
-    <t>Ilana B. Witten</t>
-  </si>
-  <si>
-    <t>Temporospatial Dynamics of the Epithelial-Mesenchymal Transition in Cancer Metastasis_ - Daniel D. Liu.xml</t>
-  </si>
-  <si>
-    <t>Daniel D. Liu</t>
-  </si>
-  <si>
-    <t>Yibin Kang Lab</t>
-  </si>
-  <si>
-    <t>Missed Connections_ A Collection of Short Stories - Rebecca Kahn.xml</t>
-  </si>
-  <si>
-    <t>Rebecca N. Kahn</t>
-  </si>
-  <si>
-    <t>Daphne E. Kalotay</t>
-  </si>
-  <si>
-    <t>Photoswitchable Protein-Protein Interactions_ Engineering Light-Sensitive DARPins - Joshua Kim.xml</t>
-  </si>
-  <si>
-    <t>Joshua S. Kim</t>
-  </si>
-  <si>
-    <t>Toettcher</t>
-  </si>
-  <si>
-    <t>Fear_ Fetish_ and FaÁade_ The Role of Privilege and Self-Curation in Educational Outcomes - Olivia Fiechter.xml</t>
   </si>
   <si>
     <t>Pricing Accelerated Share Repurchases with Lookback Options - Easton Orbe.xml</t>
@@ -684,387 +673,74 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="22" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="10.56"/>
+    <col customWidth="1" min="2" max="2" width="53.11"/>
+    <col customWidth="1" min="3" max="3" width="24.78"/>
+    <col customWidth="1" min="4" max="4" width="24.0"/>
+    <col customWidth="1" min="5" max="5" width="10.56"/>
+    <col customWidth="1" min="6" max="6" width="21.78"/>
+    <col customWidth="1" min="7" max="8" width="10.56"/>
+    <col customWidth="1" min="9" max="9" width="17.78"/>
+    <col customWidth="1" min="10" max="26" width="10.56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1114,9 +790,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2">
       <c r="A2">
-        <v>2462</v>
+        <v>2462.0</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -1125,10 +801,10 @@
         <v>17</v>
       </c>
       <c r="D2" s="1">
-        <v>41713.974305555559</v>
+        <v>43175.97430555556</v>
       </c>
       <c r="E2">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
@@ -1164,9 +840,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3">
       <c r="A3">
-        <v>1690</v>
+        <v>1690.0</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -1175,10 +851,10 @@
         <v>27</v>
       </c>
       <c r="D3" s="1">
-        <v>41720.45208333333</v>
+        <v>43182.45208333333</v>
       </c>
       <c r="E3">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -1214,9 +890,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4">
       <c r="A4">
-        <v>1953</v>
+        <v>1953.0</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -1225,10 +901,10 @@
         <v>30</v>
       </c>
       <c r="D4" s="1">
-        <v>41721.452777777777</v>
+        <v>43183.45277777778</v>
       </c>
       <c r="E4">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
@@ -1264,9 +940,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5">
       <c r="A5">
-        <v>1833</v>
+        <v>1833.0</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
@@ -1275,10 +951,10 @@
         <v>34</v>
       </c>
       <c r="D5" s="1">
-        <v>41726.488888888889</v>
+        <v>43188.48888888889</v>
       </c>
       <c r="E5">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F5" t="s">
         <v>35</v>
@@ -1314,9 +990,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6">
       <c r="A6">
-        <v>1629</v>
+        <v>1629.0</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -1325,10 +1001,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="1">
-        <v>41730.658333333333</v>
+        <v>43192.65833333333</v>
       </c>
       <c r="E6">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F6" t="s">
         <v>39</v>
@@ -1364,9 +1040,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7">
       <c r="A7">
-        <v>1575</v>
+        <v>1575.0</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -1375,10 +1051,10 @@
         <v>42</v>
       </c>
       <c r="D7" s="1">
-        <v>41731.440972222219</v>
+        <v>43193.44097222222</v>
       </c>
       <c r="E7">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F7" t="s">
         <v>43</v>
@@ -1414,9 +1090,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8">
       <c r="A8">
-        <v>2606</v>
+        <v>2606.0</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
@@ -1425,10 +1101,10 @@
         <v>30</v>
       </c>
       <c r="D8" s="1">
-        <v>41731.597222222219</v>
+        <v>43193.59722222222</v>
       </c>
       <c r="E8">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="G8" t="s">
         <v>46</v>
@@ -1461,9 +1137,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9">
-        <v>2641</v>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>1935.0</v>
       </c>
       <c r="B9" t="s">
         <v>47</v>
@@ -1472,10 +1148,10 @@
         <v>48</v>
       </c>
       <c r="D9" s="1">
-        <v>41731.61041666667</v>
+        <v>43193.61041666667</v>
       </c>
       <c r="E9">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="G9" t="s">
         <v>49</v>
@@ -1508,9 +1184,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10">
       <c r="A10">
-        <v>1821</v>
+        <v>1821.0</v>
       </c>
       <c r="B10" t="s">
         <v>50</v>
@@ -1519,10 +1195,10 @@
         <v>51</v>
       </c>
       <c r="D10" s="1">
-        <v>41736.938888888893</v>
+        <v>43198.93888888889</v>
       </c>
       <c r="E10">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F10" t="s">
         <v>52</v>
@@ -1558,9 +1234,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11">
       <c r="A11">
-        <v>2340</v>
+        <v>2340.0</v>
       </c>
       <c r="B11" t="s">
         <v>54</v>
@@ -1569,10 +1245,10 @@
         <v>55</v>
       </c>
       <c r="D11" s="1">
-        <v>41738.371527777781</v>
+        <v>43200.37152777778</v>
       </c>
       <c r="E11">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
@@ -1608,9 +1284,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12">
       <c r="A12">
-        <v>1910</v>
+        <v>1910.0</v>
       </c>
       <c r="B12" t="s">
         <v>58</v>
@@ -1619,10 +1295,10 @@
         <v>59</v>
       </c>
       <c r="D12" s="1">
-        <v>41738.469444444447</v>
+        <v>43200.46944444445</v>
       </c>
       <c r="E12">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F12" t="s">
         <v>31</v>
@@ -1631,7 +1307,7 @@
         <v>60</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I12" t="s">
         <v>61</v>
@@ -1658,9 +1334,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13">
       <c r="A13">
-        <v>2589</v>
+        <v>2589.0</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
@@ -1669,10 +1345,10 @@
         <v>65</v>
       </c>
       <c r="D13" s="1">
-        <v>41738.533333333333</v>
+        <v>43200.53333333333</v>
       </c>
       <c r="E13">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F13" t="s">
         <v>18</v>
@@ -1708,9 +1384,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14">
       <c r="A14">
-        <v>2459</v>
+        <v>2459.0</v>
       </c>
       <c r="B14" t="s">
         <v>67</v>
@@ -1719,10 +1395,10 @@
         <v>68</v>
       </c>
       <c r="D14" s="1">
-        <v>41739.00416666668</v>
+        <v>43201.00416666668</v>
       </c>
       <c r="E14">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
@@ -1758,9 +1434,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15">
       <c r="A15">
-        <v>2292</v>
+        <v>2292.0</v>
       </c>
       <c r="B15" t="s">
         <v>70</v>
@@ -1769,10 +1445,10 @@
         <v>71</v>
       </c>
       <c r="D15" s="1">
-        <v>41740.654861111107</v>
+        <v>43202.65486111111</v>
       </c>
       <c r="E15">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F15" t="s">
         <v>72</v>
@@ -1781,7 +1457,7 @@
         <v>73</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I15" t="s">
         <v>21</v>
@@ -1808,9 +1484,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16">
       <c r="A16">
-        <v>1678</v>
+        <v>1678.0</v>
       </c>
       <c r="B16" t="s">
         <v>75</v>
@@ -1819,10 +1495,10 @@
         <v>76</v>
       </c>
       <c r="D16" s="1">
-        <v>41741.036805555559</v>
+        <v>43203.03680555556</v>
       </c>
       <c r="E16">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F16" t="s">
         <v>77</v>
@@ -1831,7 +1507,7 @@
         <v>78</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="I16" t="s">
         <v>61</v>
@@ -1858,9 +1534,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17">
       <c r="A17">
-        <v>2672</v>
+        <v>2672.0</v>
       </c>
       <c r="B17" t="s">
         <v>79</v>
@@ -1869,10 +1545,10 @@
         <v>80</v>
       </c>
       <c r="D17" s="1">
-        <v>41741.44166666668</v>
+        <v>43203.44166666668</v>
       </c>
       <c r="E17">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F17" t="s">
         <v>81</v>
@@ -1908,9 +1584,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18">
       <c r="A18">
-        <v>2641</v>
+        <v>2641.0</v>
       </c>
       <c r="B18" t="s">
         <v>83</v>
@@ -1919,10 +1595,10 @@
         <v>48</v>
       </c>
       <c r="D18" s="1">
-        <v>41741.44166666668</v>
+        <v>43203.44166666668</v>
       </c>
       <c r="E18">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F18" t="s">
         <v>81</v>
@@ -1958,9 +1634,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19">
       <c r="A19">
-        <v>1565</v>
+        <v>1565.0</v>
       </c>
       <c r="B19" t="s">
         <v>85</v>
@@ -1969,10 +1645,10 @@
         <v>86</v>
       </c>
       <c r="D19" s="1">
-        <v>41741.931944444441</v>
+        <v>43203.93194444444</v>
       </c>
       <c r="E19">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F19" t="s">
         <v>56</v>
@@ -2008,9 +1684,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20">
       <c r="A20">
-        <v>1622</v>
+        <v>1622.0</v>
       </c>
       <c r="B20" t="s">
         <v>88</v>
@@ -2019,10 +1695,10 @@
         <v>89</v>
       </c>
       <c r="D20" s="1">
-        <v>41743.631249999999</v>
+        <v>43205.63125</v>
       </c>
       <c r="E20">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F20" t="s">
         <v>56</v>
@@ -2058,9 +1734,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21">
-        <v>1374</v>
+        <v>1374.0</v>
       </c>
       <c r="B21" t="s">
         <v>90</v>
@@ -2069,10 +1745,10 @@
         <v>91</v>
       </c>
       <c r="D21" s="1">
-        <v>41743.865277777782</v>
+        <v>43205.86527777778</v>
       </c>
       <c r="E21">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F21" t="s">
         <v>92</v>
@@ -2081,7 +1757,7 @@
         <v>93</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I21" t="s">
         <v>21</v>
@@ -2108,9 +1784,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22">
-        <v>2153</v>
+        <v>2153.0</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
@@ -2119,10 +1795,10 @@
         <v>95</v>
       </c>
       <c r="D22" s="1">
-        <v>41751.724305555559</v>
+        <v>43213.72430555556</v>
       </c>
       <c r="E22">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F22" t="s">
         <v>96</v>
@@ -2158,9 +1834,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23">
-        <v>1613</v>
+        <v>1895.0</v>
       </c>
       <c r="B23" t="s">
         <v>98</v>
@@ -2169,10 +1845,10 @@
         <v>99</v>
       </c>
       <c r="D23" s="1">
-        <v>41752.525000000001</v>
+        <v>43214.73055555556</v>
       </c>
       <c r="E23">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F23" t="s">
         <v>100</v>
@@ -2180,37 +1856,37 @@
       <c r="G23" t="s">
         <v>101</v>
       </c>
-      <c r="H23" t="s">
-        <v>20</v>
+      <c r="H23">
+        <v>2.0</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="J23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K23" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="L23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M23" t="s">
         <v>21</v>
       </c>
       <c r="N23" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="O23" t="s">
         <v>24</v>
       </c>
       <c r="P23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24">
-        <v>1895</v>
+        <v>1931.0</v>
       </c>
       <c r="B24" t="s">
         <v>102</v>
@@ -2219,10 +1895,10 @@
         <v>103</v>
       </c>
       <c r="D24" s="1">
-        <v>41752.730555555558</v>
+        <v>43216.57777777778</v>
       </c>
       <c r="E24">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F24" t="s">
         <v>104</v>
@@ -2230,17 +1906,17 @@
       <c r="G24" t="s">
         <v>105</v>
       </c>
-      <c r="H24">
-        <v>2</v>
+      <c r="H24" t="s">
+        <v>20</v>
       </c>
       <c r="I24" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="J24" t="s">
         <v>22</v>
       </c>
       <c r="K24" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="L24" t="s">
         <v>23</v>
@@ -2255,12 +1931,12 @@
         <v>24</v>
       </c>
       <c r="P24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25">
-        <v>1931</v>
+        <v>2199.0</v>
       </c>
       <c r="B25" t="s">
         <v>106</v>
@@ -2269,10 +1945,10 @@
         <v>107</v>
       </c>
       <c r="D25" s="1">
-        <v>41754.577777777777</v>
+        <v>43217.04930555557</v>
       </c>
       <c r="E25">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F25" t="s">
         <v>108</v>
@@ -2308,9 +1984,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26">
-        <v>2199</v>
+        <v>2686.0</v>
       </c>
       <c r="B26" t="s">
         <v>110</v>
@@ -2319,72 +1995,69 @@
         <v>111</v>
       </c>
       <c r="D26" s="1">
-        <v>41755.049305555571</v>
+        <v>43217.59027777778</v>
       </c>
       <c r="E26">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" t="s">
         <v>112</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26">
+        <v>2.0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" t="s">
+        <v>62</v>
+      </c>
+      <c r="L26" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26" t="s">
+        <v>21</v>
+      </c>
+      <c r="O26" t="s">
+        <v>24</v>
+      </c>
+      <c r="P26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27">
+        <v>1831.0</v>
+      </c>
+      <c r="B27" t="s">
         <v>113</v>
       </c>
-      <c r="H26" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" t="s">
-        <v>23</v>
-      </c>
-      <c r="M26" t="s">
-        <v>21</v>
-      </c>
-      <c r="N26" t="s">
-        <v>21</v>
-      </c>
-      <c r="O26" t="s">
-        <v>24</v>
-      </c>
-      <c r="P26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27">
-        <v>2686</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>114</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" s="1">
+        <v>43218.43958333333</v>
+      </c>
+      <c r="E27">
+        <v>2018.0</v>
+      </c>
+      <c r="G27" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="1">
-        <v>41755.590277777781</v>
-      </c>
-      <c r="E27">
-        <v>2018</v>
-      </c>
-      <c r="F27" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" t="s">
-        <v>116</v>
-      </c>
       <c r="H27">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I27" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="J27" t="s">
         <v>22</v>
@@ -2405,30 +2078,33 @@
         <v>24</v>
       </c>
       <c r="P27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28">
-        <v>1831</v>
+        <v>1880.0</v>
       </c>
       <c r="B28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" t="s">
         <v>117</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" s="1">
+        <v>43220.02152777778</v>
+      </c>
+      <c r="E28">
+        <v>2018.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="1">
-        <v>41756.439583333333</v>
-      </c>
-      <c r="E28">
-        <v>2018</v>
-      </c>
-      <c r="G28" t="s">
-        <v>119</v>
-      </c>
       <c r="H28">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I28" t="s">
         <v>21</v>
@@ -2455,30 +2131,30 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29">
-        <v>1880</v>
+        <v>1613.0</v>
       </c>
       <c r="B29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" t="s">
         <v>120</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" s="1">
+        <v>43221.99305555555</v>
+      </c>
+      <c r="E29">
+        <v>2018.0</v>
+      </c>
+      <c r="F29" t="s">
         <v>121</v>
-      </c>
-      <c r="D29" s="1">
-        <v>41758.021527777782</v>
-      </c>
-      <c r="E29">
-        <v>2018</v>
-      </c>
-      <c r="F29" t="s">
-        <v>112</v>
       </c>
       <c r="G29" t="s">
         <v>122</v>
       </c>
-      <c r="H29">
-        <v>2</v>
+      <c r="H29" s="2">
+        <v>75.0</v>
       </c>
       <c r="I29" t="s">
         <v>21</v>
@@ -2490,13 +2166,13 @@
         <v>62</v>
       </c>
       <c r="L29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M29" t="s">
         <v>21</v>
       </c>
       <c r="N29" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="O29" t="s">
         <v>24</v>
@@ -2505,30 +2181,30 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30">
-        <v>1613</v>
+        <v>2145.0</v>
       </c>
       <c r="B30" t="s">
         <v>123</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="D30" s="1">
-        <v>41759.993055555547</v>
+        <v>43227.48541666667</v>
       </c>
       <c r="E30">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F30" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="G30" t="s">
-        <v>101</v>
-      </c>
-      <c r="H30">
-        <v>2</v>
+        <v>126</v>
+      </c>
+      <c r="H30" t="s">
+        <v>20</v>
       </c>
       <c r="I30" t="s">
         <v>21</v>
@@ -2537,45 +2213,45 @@
         <v>22</v>
       </c>
       <c r="K30" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="L30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M30" t="s">
         <v>21</v>
       </c>
       <c r="N30" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="O30" t="s">
         <v>24</v>
       </c>
       <c r="P30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31">
-        <v>2145</v>
+        <v>2341.0</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="1">
+        <v>43227.73402777778</v>
+      </c>
+      <c r="E31">
+        <v>2018.0</v>
+      </c>
+      <c r="F31" t="s">
         <v>125</v>
       </c>
-      <c r="D31" s="1">
-        <v>41765.48541666667</v>
-      </c>
-      <c r="E31">
-        <v>2018</v>
-      </c>
-      <c r="F31" t="s">
-        <v>126</v>
-      </c>
       <c r="G31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H31" t="s">
         <v>20</v>
@@ -2605,27 +2281,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32">
-        <v>2341</v>
+        <v>2578.0</v>
       </c>
       <c r="B32" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D32" s="1">
-        <v>41765.734027777777</v>
+        <v>43227.92013888889</v>
       </c>
       <c r="E32">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F32" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="G32" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H32" t="s">
         <v>20</v>
@@ -2655,27 +2331,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33">
-        <v>2578</v>
+        <v>1943.0</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D33" s="1">
-        <v>41765.920138888891</v>
+        <v>43228.00416666668</v>
       </c>
       <c r="E33">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F33" t="s">
-        <v>133</v>
+        <v>31</v>
       </c>
       <c r="G33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H33" t="s">
         <v>20</v>
@@ -2705,39 +2381,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34">
-        <v>1943</v>
+        <v>2103.0</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D34" s="1">
-        <v>41766.00416666668</v>
+        <v>43229.575</v>
       </c>
       <c r="E34">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="G34" t="s">
-        <v>137</v>
-      </c>
-      <c r="H34" t="s">
-        <v>20</v>
+        <v>140</v>
+      </c>
+      <c r="H34">
+        <v>2.0</v>
       </c>
       <c r="I34" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="J34" t="s">
         <v>22</v>
       </c>
       <c r="K34" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="L34" t="s">
         <v>23</v>
@@ -2752,33 +2428,33 @@
         <v>24</v>
       </c>
       <c r="P34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35">
-        <v>2103</v>
+        <v>1872.0</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D35" s="1">
-        <v>41767.574999999997</v>
+        <v>43229.60555555556</v>
       </c>
       <c r="E35">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F35" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="G35" t="s">
-        <v>141</v>
-      </c>
-      <c r="H35">
-        <v>2</v>
+        <v>143</v>
+      </c>
+      <c r="H35" s="2">
+        <v>5.0</v>
       </c>
       <c r="I35" t="s">
         <v>61</v>
@@ -2805,30 +2481,30 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36">
-        <v>1872</v>
+        <v>2222.0</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D36" s="1">
-        <v>41767.605555555558</v>
+        <v>43230.96875</v>
       </c>
       <c r="E36">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F36" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="G36" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H36">
-        <v>2</v>
+        <v>1.0</v>
       </c>
       <c r="I36" t="s">
         <v>61</v>
@@ -2855,30 +2531,30 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37">
-        <v>2222</v>
+        <v>1785.0</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D37" s="1">
-        <v>41768.96875</v>
+        <v>43233.54583333333</v>
       </c>
       <c r="E37">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F37" t="s">
+        <v>139</v>
+      </c>
+      <c r="G37" t="s">
         <v>140</v>
       </c>
-      <c r="G37" t="s">
-        <v>147</v>
-      </c>
       <c r="H37">
-        <v>1</v>
+        <v>2.0</v>
       </c>
       <c r="I37" t="s">
         <v>61</v>
@@ -2905,33 +2581,33 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38">
-        <v>1785</v>
+        <v>2162.0</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D38" s="1">
-        <v>41771.54583333333</v>
+        <v>43233.54722222222</v>
       </c>
       <c r="E38">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F38" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="G38" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I38" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="J38" t="s">
         <v>22</v>
@@ -2952,33 +2628,33 @@
         <v>24</v>
       </c>
       <c r="P38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39">
-        <v>2162</v>
+        <v>1836.0</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D39" s="1">
-        <v>41771.547222222223</v>
+        <v>43235.69444444445</v>
       </c>
       <c r="E39">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F39" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="G39" t="s">
-        <v>116</v>
-      </c>
-      <c r="H39">
-        <v>2</v>
+        <v>153</v>
+      </c>
+      <c r="H39" t="s">
+        <v>20</v>
       </c>
       <c r="I39" t="s">
         <v>21</v>
@@ -2987,101 +2663,101 @@
         <v>22</v>
       </c>
       <c r="K39" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" t="s">
+        <v>21</v>
+      </c>
+      <c r="N39" t="s">
+        <v>21</v>
+      </c>
+      <c r="O39" t="s">
+        <v>24</v>
+      </c>
+      <c r="P39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40">
+        <v>2169.0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" t="s">
+        <v>155</v>
+      </c>
+      <c r="D40" s="1">
+        <v>43235.93611111111</v>
+      </c>
+      <c r="E40">
+        <v>2018.0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>139</v>
+      </c>
+      <c r="G40" t="s">
+        <v>140</v>
+      </c>
+      <c r="H40">
+        <v>2.0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" t="s">
         <v>62</v>
       </c>
-      <c r="L39" t="s">
-        <v>23</v>
-      </c>
-      <c r="M39" t="s">
-        <v>21</v>
-      </c>
-      <c r="N39" t="s">
-        <v>21</v>
-      </c>
-      <c r="O39" t="s">
-        <v>24</v>
-      </c>
-      <c r="P39" t="s">
+      <c r="L40" t="s">
+        <v>23</v>
+      </c>
+      <c r="M40" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40" t="s">
+        <v>21</v>
+      </c>
+      <c r="O40" t="s">
+        <v>24</v>
+      </c>
+      <c r="P40" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
-      <c r="A40">
-        <v>1836</v>
-      </c>
-      <c r="B40" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" t="s">
-        <v>153</v>
-      </c>
-      <c r="D40" s="1">
-        <v>41773.694444444453</v>
-      </c>
-      <c r="E40">
-        <v>2018</v>
-      </c>
-      <c r="F40" t="s">
-        <v>56</v>
-      </c>
-      <c r="G40" t="s">
-        <v>154</v>
-      </c>
-      <c r="H40" t="s">
-        <v>20</v>
-      </c>
-      <c r="I40" t="s">
-        <v>21</v>
-      </c>
-      <c r="J40" t="s">
-        <v>22</v>
-      </c>
-      <c r="K40" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" t="s">
-        <v>23</v>
-      </c>
-      <c r="M40" t="s">
-        <v>21</v>
-      </c>
-      <c r="N40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O40" t="s">
-        <v>24</v>
-      </c>
-      <c r="P40" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41">
-        <v>2169</v>
+        <v>1556.0</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C41" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D41" s="1">
-        <v>41773.936111111107</v>
+        <v>43236.59583333333</v>
       </c>
       <c r="E41">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F41" t="s">
+        <v>139</v>
+      </c>
+      <c r="G41" t="s">
         <v>140</v>
       </c>
-      <c r="G41" t="s">
-        <v>141</v>
-      </c>
       <c r="H41">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I41" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="J41" t="s">
         <v>22</v>
@@ -3102,42 +2778,42 @@
         <v>24</v>
       </c>
       <c r="P41" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
       <c r="A42">
-        <v>1556</v>
+        <v>2223.0</v>
       </c>
       <c r="B42" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D42" s="1">
-        <v>41774.595833333333</v>
+        <v>43236.68611111111</v>
       </c>
       <c r="E42">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F42" t="s">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="G42" t="s">
-        <v>141</v>
-      </c>
-      <c r="H42">
-        <v>2</v>
+        <v>160</v>
+      </c>
+      <c r="H42" t="s">
+        <v>20</v>
       </c>
       <c r="I42" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="J42" t="s">
         <v>22</v>
       </c>
       <c r="K42" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="L42" t="s">
         <v>23</v>
@@ -3152,30 +2828,30 @@
         <v>24</v>
       </c>
       <c r="P42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
       <c r="A43">
-        <v>2223</v>
+        <v>1904.0</v>
       </c>
       <c r="B43" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D43" s="1">
-        <v>41774.686111111107</v>
+        <v>43237.64444444444</v>
       </c>
       <c r="E43">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F43" t="s">
         <v>35</v>
       </c>
       <c r="G43" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H43" t="s">
         <v>20</v>
@@ -3205,27 +2881,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" ht="15.75" customHeight="1">
       <c r="A44">
-        <v>1904</v>
+        <v>2620.0</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D44" s="1">
-        <v>41775.644444444442</v>
+        <v>43241.63402777778</v>
       </c>
       <c r="E44">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F44" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G44" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H44" t="s">
         <v>20</v>
@@ -3255,140 +2931,140 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" ht="15.75" customHeight="1">
       <c r="A45">
-        <v>2620</v>
+        <v>2159.0</v>
       </c>
       <c r="B45" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C45" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D45" s="1">
-        <v>41779.634027777778</v>
+        <v>43241.70833333334</v>
       </c>
       <c r="E45">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F45" t="s">
+        <v>169</v>
+      </c>
+      <c r="G45" t="s">
+        <v>170</v>
+      </c>
+      <c r="H45">
+        <v>2.0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" t="s">
+        <v>22</v>
+      </c>
+      <c r="K45" t="s">
+        <v>62</v>
+      </c>
+      <c r="L45" t="s">
+        <v>23</v>
+      </c>
+      <c r="M45" t="s">
+        <v>21</v>
+      </c>
+      <c r="N45" t="s">
+        <v>21</v>
+      </c>
+      <c r="O45" t="s">
+        <v>24</v>
+      </c>
+      <c r="P45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46">
+        <v>2287.0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" t="s">
+        <v>172</v>
+      </c>
+      <c r="D46" s="1">
+        <v>43242.59930555556</v>
+      </c>
+      <c r="E46">
+        <v>2018.0</v>
+      </c>
+      <c r="F46" t="s">
         <v>56</v>
       </c>
-      <c r="G45" t="s">
-        <v>167</v>
-      </c>
-      <c r="H45" t="s">
-        <v>20</v>
-      </c>
-      <c r="I45" t="s">
-        <v>21</v>
-      </c>
-      <c r="J45" t="s">
-        <v>22</v>
-      </c>
-      <c r="K45" t="s">
-        <v>20</v>
-      </c>
-      <c r="L45" t="s">
-        <v>23</v>
-      </c>
-      <c r="M45" t="s">
-        <v>21</v>
-      </c>
-      <c r="N45" t="s">
-        <v>21</v>
-      </c>
-      <c r="O45" t="s">
-        <v>24</v>
-      </c>
-      <c r="P45" t="s">
+      <c r="G46" t="s">
+        <v>173</v>
+      </c>
+      <c r="H46" t="s">
+        <v>20</v>
+      </c>
+      <c r="I46" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K46" t="s">
+        <v>20</v>
+      </c>
+      <c r="L46" t="s">
+        <v>23</v>
+      </c>
+      <c r="M46" t="s">
+        <v>21</v>
+      </c>
+      <c r="N46" t="s">
+        <v>21</v>
+      </c>
+      <c r="O46" t="s">
+        <v>24</v>
+      </c>
+      <c r="P46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
-      <c r="A46">
-        <v>2159</v>
-      </c>
-      <c r="B46" t="s">
-        <v>168</v>
-      </c>
-      <c r="C46" t="s">
-        <v>169</v>
-      </c>
-      <c r="D46" s="1">
-        <v>41779.708333333343</v>
-      </c>
-      <c r="E46">
-        <v>2018</v>
-      </c>
-      <c r="F46" t="s">
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47">
+        <v>1918.0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" t="s">
+        <v>175</v>
+      </c>
+      <c r="D47" s="1">
+        <v>43243.60208333333</v>
+      </c>
+      <c r="E47">
+        <v>2018.0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>176</v>
+      </c>
+      <c r="G47" t="s">
         <v>170</v>
       </c>
-      <c r="G46" t="s">
-        <v>171</v>
-      </c>
-      <c r="H46">
-        <v>2</v>
-      </c>
-      <c r="I46" t="s">
-        <v>21</v>
-      </c>
-      <c r="J46" t="s">
-        <v>22</v>
-      </c>
-      <c r="K46" t="s">
+      <c r="H47">
+        <v>1.0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>61</v>
+      </c>
+      <c r="J47" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" t="s">
         <v>62</v>
       </c>
-      <c r="L46" t="s">
-        <v>23</v>
-      </c>
-      <c r="M46" t="s">
-        <v>21</v>
-      </c>
-      <c r="N46" t="s">
-        <v>21</v>
-      </c>
-      <c r="O46" t="s">
-        <v>24</v>
-      </c>
-      <c r="P46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16">
-      <c r="A47">
-        <v>2287</v>
-      </c>
-      <c r="B47" t="s">
-        <v>172</v>
-      </c>
-      <c r="C47" t="s">
-        <v>173</v>
-      </c>
-      <c r="D47" s="1">
-        <v>41780.599305555559</v>
-      </c>
-      <c r="E47">
-        <v>2018</v>
-      </c>
-      <c r="F47" t="s">
-        <v>56</v>
-      </c>
-      <c r="G47" t="s">
-        <v>174</v>
-      </c>
-      <c r="H47" t="s">
-        <v>20</v>
-      </c>
-      <c r="I47" t="s">
-        <v>21</v>
-      </c>
-      <c r="J47" t="s">
-        <v>22</v>
-      </c>
-      <c r="K47" t="s">
-        <v>20</v>
-      </c>
       <c r="L47" t="s">
         <v>23</v>
       </c>
@@ -3402,80 +3078,80 @@
         <v>24</v>
       </c>
       <c r="P47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48">
+        <v>2124.0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" t="s">
+        <v>178</v>
+      </c>
+      <c r="D48" s="1">
+        <v>43245.46875</v>
+      </c>
+      <c r="E48">
+        <v>2018.0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" t="s">
+        <v>179</v>
+      </c>
+      <c r="H48" t="s">
+        <v>20</v>
+      </c>
+      <c r="I48" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K48" t="s">
+        <v>20</v>
+      </c>
+      <c r="L48" t="s">
+        <v>23</v>
+      </c>
+      <c r="M48" t="s">
+        <v>21</v>
+      </c>
+      <c r="N48" t="s">
+        <v>21</v>
+      </c>
+      <c r="O48" t="s">
+        <v>24</v>
+      </c>
+      <c r="P48" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
-      <c r="A48">
-        <v>1918</v>
-      </c>
-      <c r="B48" t="s">
-        <v>175</v>
-      </c>
-      <c r="C48" t="s">
-        <v>176</v>
-      </c>
-      <c r="D48" s="1">
-        <v>41781.602083333331</v>
-      </c>
-      <c r="E48">
-        <v>2018</v>
-      </c>
-      <c r="F48" t="s">
-        <v>177</v>
-      </c>
-      <c r="G48" t="s">
-        <v>171</v>
-      </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
-      <c r="I48" t="s">
-        <v>61</v>
-      </c>
-      <c r="J48" t="s">
-        <v>22</v>
-      </c>
-      <c r="K48" t="s">
-        <v>62</v>
-      </c>
-      <c r="L48" t="s">
-        <v>23</v>
-      </c>
-      <c r="M48" t="s">
-        <v>21</v>
-      </c>
-      <c r="N48" t="s">
-        <v>21</v>
-      </c>
-      <c r="O48" t="s">
-        <v>24</v>
-      </c>
-      <c r="P48" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16">
+    <row r="49" ht="15.75" customHeight="1">
       <c r="A49">
-        <v>2124</v>
+        <v>1528.0</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C49" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D49" s="1">
-        <v>41783.46875</v>
+        <v>43245.68611111111</v>
       </c>
       <c r="E49">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F49" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="G49" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H49" t="s">
         <v>20</v>
@@ -3505,27 +3181,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" ht="15.75" customHeight="1">
       <c r="A50">
-        <v>1528</v>
+        <v>2329.0</v>
       </c>
       <c r="B50" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C50" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D50" s="1">
-        <v>41783.686111111107</v>
+        <v>43245.72430555556</v>
       </c>
       <c r="E50">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F50" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="G50" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H50" t="s">
         <v>20</v>
@@ -3555,39 +3231,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" ht="15.75" customHeight="1">
       <c r="A51">
-        <v>2329</v>
+        <v>1322.0</v>
       </c>
       <c r="B51" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C51" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D51" s="1">
-        <v>41783.724305555559</v>
+        <v>43249.60208333333</v>
       </c>
       <c r="E51">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F51" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G51" t="s">
-        <v>186</v>
-      </c>
-      <c r="H51" t="s">
-        <v>20</v>
+        <v>188</v>
+      </c>
+      <c r="H51">
+        <v>2.0</v>
       </c>
       <c r="I51" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="J51" t="s">
         <v>22</v>
       </c>
       <c r="K51" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="L51" t="s">
         <v>23</v>
@@ -3602,92 +3278,92 @@
         <v>24</v>
       </c>
       <c r="P51" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
       <c r="A52">
-        <v>1322</v>
+        <v>2518.0</v>
       </c>
       <c r="B52" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C52" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D52" s="1">
-        <v>41787.602083333331</v>
+        <v>43252.70833333334</v>
       </c>
       <c r="E52">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F52" t="s">
-        <v>96</v>
+        <v>169</v>
       </c>
       <c r="G52" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H52">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="I52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" t="s">
+        <v>22</v>
+      </c>
+      <c r="K52" t="s">
+        <v>192</v>
+      </c>
+      <c r="L52" t="s">
+        <v>24</v>
+      </c>
+      <c r="M52" t="s">
+        <v>21</v>
+      </c>
+      <c r="N52" t="s">
         <v>61</v>
       </c>
-      <c r="J52" t="s">
-        <v>22</v>
-      </c>
-      <c r="K52" t="s">
-        <v>62</v>
-      </c>
-      <c r="L52" t="s">
-        <v>23</v>
-      </c>
-      <c r="M52" t="s">
-        <v>21</v>
-      </c>
-      <c r="N52" t="s">
-        <v>21</v>
-      </c>
       <c r="O52" t="s">
         <v>24</v>
       </c>
       <c r="P52" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
       <c r="A53">
-        <v>2518</v>
+        <v>2133.0</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C53" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D53" s="1">
-        <v>41790.708333333343</v>
+        <v>43254.91736111111</v>
       </c>
       <c r="E53">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F53" t="s">
+        <v>169</v>
+      </c>
+      <c r="G53" t="s">
         <v>170</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53">
+        <v>2.0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>61</v>
+      </c>
+      <c r="J53" t="s">
+        <v>22</v>
+      </c>
+      <c r="K53" t="s">
         <v>192</v>
-      </c>
-      <c r="H53">
-        <v>2</v>
-      </c>
-      <c r="I53" t="s">
-        <v>21</v>
-      </c>
-      <c r="J53" t="s">
-        <v>22</v>
-      </c>
-      <c r="K53" t="s">
-        <v>193</v>
       </c>
       <c r="L53" t="s">
         <v>24</v>
@@ -3702,33 +3378,33 @@
         <v>24</v>
       </c>
       <c r="P53" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
       <c r="A54">
-        <v>2133</v>
+        <v>1820.0</v>
       </c>
       <c r="B54" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C54" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D54" s="1">
-        <v>41792.917361111111</v>
+        <v>43254.99166666667</v>
       </c>
       <c r="E54">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F54" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="G54" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="H54">
-        <v>2</v>
+        <v>1.0</v>
       </c>
       <c r="I54" t="s">
         <v>61</v>
@@ -3737,7 +3413,7 @@
         <v>22</v>
       </c>
       <c r="K54" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L54" t="s">
         <v>24</v>
@@ -3755,30 +3431,30 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" ht="15.75" customHeight="1">
       <c r="A55">
-        <v>1820</v>
+        <v>1321.0</v>
       </c>
       <c r="B55" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C55" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D55" s="1">
-        <v>41792.991666666669</v>
+        <v>43255.39236111111</v>
       </c>
       <c r="E55">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F55" t="s">
-        <v>133</v>
+        <v>176</v>
       </c>
       <c r="G55" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>2.0</v>
       </c>
       <c r="I55" t="s">
         <v>61</v>
@@ -3787,7 +3463,7 @@
         <v>22</v>
       </c>
       <c r="K55" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L55" t="s">
         <v>24</v>
@@ -3805,77 +3481,77 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" ht="15.75" customHeight="1">
       <c r="A56">
-        <v>1321</v>
+        <v>2230.0</v>
       </c>
       <c r="B56" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C56" t="s">
+        <v>202</v>
+      </c>
+      <c r="D56" s="1">
+        <v>43255.51875</v>
+      </c>
+      <c r="E56">
+        <v>2018.0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>176</v>
+      </c>
+      <c r="G56" t="s">
         <v>200</v>
       </c>
-      <c r="D56" s="1">
-        <v>41793.392361111109</v>
-      </c>
-      <c r="E56">
-        <v>2018</v>
-      </c>
-      <c r="F56" t="s">
-        <v>177</v>
-      </c>
-      <c r="G56" t="s">
-        <v>201</v>
-      </c>
-      <c r="H56">
-        <v>2</v>
+      <c r="H56" t="s">
+        <v>20</v>
       </c>
       <c r="I56" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="J56" t="s">
         <v>22</v>
       </c>
       <c r="K56" t="s">
-        <v>193</v>
+        <v>20</v>
       </c>
       <c r="L56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M56" t="s">
         <v>21</v>
       </c>
       <c r="N56" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="O56" t="s">
         <v>24</v>
       </c>
       <c r="P56" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
       <c r="A57">
-        <v>2230</v>
+        <v>1306.0</v>
       </c>
       <c r="B57" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C57" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D57" s="1">
-        <v>41793.518750000003</v>
+        <v>43255.57916666667</v>
       </c>
       <c r="E57">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F57" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
       <c r="G57" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="H57" t="s">
         <v>20</v>
@@ -3905,80 +3581,80 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" ht="15.75" customHeight="1">
       <c r="A58">
-        <v>1306</v>
+        <v>2404.0</v>
       </c>
       <c r="B58" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C58" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D58" s="1">
-        <v>41793.57916666667</v>
+        <v>43256.67847222222</v>
       </c>
       <c r="E58">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F58" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="G58" t="s">
-        <v>206</v>
-      </c>
-      <c r="H58" t="s">
-        <v>20</v>
+        <v>208</v>
+      </c>
+      <c r="H58">
+        <v>1.0</v>
       </c>
       <c r="I58" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="J58" t="s">
         <v>22</v>
       </c>
       <c r="K58" t="s">
-        <v>20</v>
+        <v>192</v>
       </c>
       <c r="L58" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M58" t="s">
         <v>21</v>
       </c>
       <c r="N58" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="O58" t="s">
         <v>24</v>
       </c>
       <c r="P58" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
       <c r="A59">
-        <v>2404</v>
+        <v>1698.0</v>
       </c>
       <c r="B59" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C59" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D59" s="1">
-        <v>41794.678472222222</v>
+        <v>43257.58263888889</v>
       </c>
       <c r="E59">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F59" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="G59" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>2.0</v>
       </c>
       <c r="I59" t="s">
         <v>61</v>
@@ -3987,16 +3663,16 @@
         <v>22</v>
       </c>
       <c r="K59" t="s">
-        <v>193</v>
+        <v>62</v>
       </c>
       <c r="L59" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M59" t="s">
         <v>21</v>
       </c>
       <c r="N59" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="O59" t="s">
         <v>24</v>
@@ -4005,39 +3681,39 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" ht="15.75" customHeight="1">
       <c r="A60">
-        <v>1698</v>
+        <v>1776.0</v>
       </c>
       <c r="B60" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C60" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D60" s="1">
-        <v>41795.582638888889</v>
+        <v>43260.15138888889</v>
       </c>
       <c r="E60">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F60" t="s">
-        <v>112</v>
+        <v>214</v>
       </c>
       <c r="G60" t="s">
-        <v>212</v>
-      </c>
-      <c r="H60">
-        <v>2</v>
+        <v>215</v>
+      </c>
+      <c r="H60" t="s">
+        <v>20</v>
       </c>
       <c r="I60" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="J60" t="s">
         <v>22</v>
       </c>
       <c r="K60" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="L60" t="s">
         <v>23</v>
@@ -4052,30 +3728,30 @@
         <v>24</v>
       </c>
       <c r="P60" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
       <c r="A61">
-        <v>1776</v>
+        <v>2565.0</v>
       </c>
       <c r="B61" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C61" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D61" s="1">
-        <v>41798.151388888888</v>
+        <v>43293.78611111111</v>
       </c>
       <c r="E61">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="F61" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="G61" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H61" t="s">
         <v>20</v>
@@ -4105,62 +3781,948 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
-      <c r="A62">
-        <v>2565</v>
-      </c>
-      <c r="B62" t="s">
-        <v>217</v>
-      </c>
-      <c r="C62" t="s">
-        <v>218</v>
-      </c>
-      <c r="D62" s="1">
-        <v>41831.786111111112</v>
-      </c>
-      <c r="E62">
-        <v>2018</v>
-      </c>
-      <c r="F62" t="s">
-        <v>170</v>
-      </c>
-      <c r="G62" t="s">
-        <v>219</v>
-      </c>
-      <c r="H62" t="s">
-        <v>20</v>
-      </c>
-      <c r="I62" t="s">
-        <v>21</v>
-      </c>
-      <c r="J62" t="s">
-        <v>22</v>
-      </c>
-      <c r="K62" t="s">
-        <v>20</v>
-      </c>
-      <c r="L62" t="s">
-        <v>23</v>
-      </c>
-      <c r="M62" t="s">
-        <v>21</v>
-      </c>
-      <c r="N62" t="s">
-        <v>21</v>
-      </c>
-      <c r="O62" t="s">
-        <v>24</v>
-      </c>
-      <c r="P62" t="s">
-        <v>25</v>
-      </c>
-    </row>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <printOptions/>
+  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>